<commit_message>
health_slider penyakit kritis 3x slide added (missing B4)
</commit_message>
<xml_diff>
--- a/.format input excel/Flexi Health Input Data.xlsx
+++ b/.format input excel/Flexi Health Input Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\E2U_VP\.format input excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F3BBF4-A2F5-4B8D-B1C8-F81CC82014D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F17980-6F85-466F-919D-CE4E2A264952}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="1628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="1629">
   <si>
     <t>gender</t>
   </si>
@@ -4906,6 +4906,9 @@
   </si>
   <si>
     <t>CY27</t>
+  </si>
+  <si>
+    <t>3x Slide</t>
   </si>
 </sst>
 </file>
@@ -5843,8 +5846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6075,7 +6078,7 @@
         <v>123</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>123</v>
+        <v>1628</v>
       </c>
       <c r="Q2" t="s">
         <v>72</v>
@@ -6190,7 +6193,7 @@
       <formula1>"Tidak Menggunakan Slider,1x Slide,2x Slide"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{81C15734-9987-461F-82CF-F1B071EE9E86}">
-      <formula1>"Tidak Menggunakan Slider,1x Slide,2x Slide,Max"</formula1>
+      <formula1>"Tidak Menggunakan Slider,1x Slide,2x Slide,3x Slide,Max"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>